<commit_message>
New script for ROMS temp data; updated temp in intrasp CEATTLE input
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_280310.xlsx
+++ b/data/hake_intrasp_280310.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D92EB3D-1861-6B41-B82E-625F3E24B577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7851E97F-C605-2641-AC3F-1348AD7D4FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="42700" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8680" yWindow="500" windowWidth="38400" windowHeight="42700" firstSheet="5" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1564,7 +1564,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1576,6 +1576,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1601,7 +1608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1613,6 +1620,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14271,7 +14279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
@@ -14603,10 +14611,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14619,316 +14627,324 @@
         <v>488</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1980</v>
       </c>
-      <c r="B2">
-        <v>5.23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="7">
+        <v>7.7910786500000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1981</v>
       </c>
-      <c r="B3">
-        <v>6.13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="7">
+        <v>7.9302527500000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1982</v>
       </c>
-      <c r="B4">
-        <v>4.4400000000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="7">
+        <v>7.7663626399999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1983</v>
       </c>
-      <c r="B5">
-        <v>5.33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="7">
+        <v>8.3381739100000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1984</v>
       </c>
-      <c r="B6">
-        <v>5.04</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="7">
+        <v>7.7257362599999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1985</v>
       </c>
-      <c r="B7">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="7">
+        <v>7.5189010999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1986</v>
       </c>
-      <c r="B8">
-        <v>5.0599999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="7">
+        <v>7.7015434799999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1987</v>
       </c>
-      <c r="B9">
-        <v>5.87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="7">
+        <v>7.9614065900000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1988</v>
       </c>
-      <c r="B10">
-        <v>5.18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="7">
+        <v>7.54096703</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1989</v>
       </c>
-      <c r="B11">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="7">
+        <v>7.4454456499999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1990</v>
       </c>
-      <c r="B12">
-        <v>4.46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="7">
+        <v>7.6304835200000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1991</v>
       </c>
-      <c r="B13">
-        <v>6.62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="7">
+        <v>7.3921977999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1992</v>
       </c>
-      <c r="B14">
-        <v>5.15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="7">
+        <v>8.0989565199999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1993</v>
       </c>
-      <c r="B15">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="7">
+        <v>7.6743296699999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1994</v>
       </c>
-      <c r="B16">
-        <v>4.72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="7">
+        <v>7.6574285700000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1995</v>
       </c>
-      <c r="B17">
-        <v>4.3499999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="7">
+        <v>7.7381758200000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1996</v>
       </c>
-      <c r="B18">
-        <v>4.79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="7">
+        <v>7.7203152199999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1997</v>
       </c>
-      <c r="B19">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="7">
+        <v>8.1091318700000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1998</v>
       </c>
-      <c r="B20">
-        <v>5.92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="7">
+        <v>8.1201428599999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1999</v>
       </c>
-      <c r="B21">
-        <v>4.8499999999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="7">
+        <v>7.33834783</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2000</v>
       </c>
-      <c r="B22">
-        <v>4.88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="7">
+        <v>7.4241428599999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2001</v>
       </c>
-      <c r="B23">
-        <v>5.19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="7">
+        <v>7.0958131900000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2002</v>
       </c>
-      <c r="B24">
-        <v>4.54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="7">
+        <v>7.2639239099999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2003</v>
       </c>
-      <c r="B25">
-        <v>5.54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="7">
+        <v>7.5445054899999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2004</v>
       </c>
-      <c r="B26">
-        <v>4.95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="7">
+        <v>7.64548352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2005</v>
       </c>
-      <c r="B27">
-        <v>5.17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="7">
+        <v>7.8828369599999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2006</v>
       </c>
-      <c r="B28">
-        <v>5.03</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="7">
+        <v>7.7766813199999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2007</v>
       </c>
-      <c r="B29">
-        <v>4.46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="7">
+        <v>7.4721978</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2008</v>
       </c>
-      <c r="B30">
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="7">
+        <v>7.1410434800000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2009</v>
       </c>
-      <c r="B31">
-        <v>4.0199999999999996</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B31" s="7">
+        <v>7.20131868</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2010</v>
       </c>
-      <c r="B32">
-        <v>5.46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B32" s="7">
+        <v>7.4271111100000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2011</v>
       </c>
-      <c r="B33">
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="7">
+        <v>7.4726153799999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2012</v>
       </c>
-      <c r="B34">
-        <v>4.41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="7">
+        <v>7.2943695699999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2013</v>
       </c>
-      <c r="B35">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="7">
+        <v>7.0181098899999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2014</v>
       </c>
-      <c r="B36">
-        <v>5.1100000000000003</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="7">
+        <v>7.4749340699999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2015</v>
       </c>
-      <c r="B37">
-        <v>6.17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="7">
+        <v>7.5457142900000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2016</v>
       </c>
-      <c r="B38">
-        <v>5.79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="7">
+        <v>7.3323152199999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2017</v>
       </c>
-      <c r="B39">
-        <v>5.15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="7">
+        <v>7.3101318700000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2018</v>
       </c>
-      <c r="B40">
-        <v>5.47</v>
+      <c r="B40" s="7">
+        <v>7.4305384600000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2019</v>
+      </c>
+      <c r="B41" s="7">
+        <v>7.3799565200000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>